<commit_message>
changed day_count limit to quit
</commit_message>
<xml_diff>
--- a/simulationdata.xlsx
+++ b/simulationdata.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B101"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -447,10 +447,10 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>5.2</v>
+        <v>5.6</v>
       </c>
       <c r="B2" t="n">
-        <v>5.6</v>
+        <v>4.8</v>
       </c>
     </row>
     <row r="3">
@@ -463,10 +463,10 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>5.6</v>
+        <v>6</v>
       </c>
       <c r="B4" t="n">
-        <v>6.4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5">
@@ -479,7 +479,7 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>6.4</v>
+        <v>6.8</v>
       </c>
       <c r="B6" t="n">
         <v>6.8</v>
@@ -487,23 +487,23 @@
     </row>
     <row r="7">
       <c r="A7" t="n">
+        <v>7.4</v>
+      </c>
+      <c r="B7" t="n">
         <v>7</v>
-      </c>
-      <c r="B7" t="n">
-        <v>6.6</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>7.2</v>
+        <v>7.6</v>
       </c>
       <c r="B8" t="n">
-        <v>7.2</v>
+        <v>7.6</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>7.4</v>
+        <v>8.199999999999999</v>
       </c>
       <c r="B9" t="n">
         <v>7.8</v>
@@ -511,18 +511,738 @@
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>8</v>
+        <v>8.4</v>
       </c>
       <c r="B10" t="n">
-        <v>7.6</v>
+        <v>8.4</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>8.199999999999999</v>
+        <v>8.6</v>
       </c>
       <c r="B11" t="n">
-        <v>8.199999999999999</v>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>9.199999999999999</v>
+      </c>
+      <c r="B12" t="n">
+        <v>8.800000000000001</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>9.4</v>
+      </c>
+      <c r="B13" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>10</v>
+      </c>
+      <c r="B14" t="n">
+        <v>9.199999999999999</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>10.2</v>
+      </c>
+      <c r="B15" t="n">
+        <v>9.800000000000001</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>10.4</v>
+      </c>
+      <c r="B16" t="n">
+        <v>10.4</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>11</v>
+      </c>
+      <c r="B17" t="n">
+        <v>10.6</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>11.2</v>
+      </c>
+      <c r="B18" t="n">
+        <v>11.2</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>11.8</v>
+      </c>
+      <c r="B19" t="n">
+        <v>11.4</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>12</v>
+      </c>
+      <c r="B20" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>12.2</v>
+      </c>
+      <c r="B21" t="n">
+        <v>12.6</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>12.4</v>
+      </c>
+      <c r="B22" t="n">
+        <v>12.8</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>12.6</v>
+      </c>
+      <c r="B23" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>12.8</v>
+      </c>
+      <c r="B24" t="n">
+        <v>13.6</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>13.4</v>
+      </c>
+      <c r="B25" t="n">
+        <v>13.8</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>13.6</v>
+      </c>
+      <c r="B26" t="n">
+        <v>14.4</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>14.2</v>
+      </c>
+      <c r="B27" t="n">
+        <v>14.6</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>14.4</v>
+      </c>
+      <c r="B28" t="n">
+        <v>14.8</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>14.6</v>
+      </c>
+      <c r="B29" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>14.8</v>
+      </c>
+      <c r="B30" t="n">
+        <v>15.2</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>15</v>
+      </c>
+      <c r="B31" t="n">
+        <v>15.8</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>15.2</v>
+      </c>
+      <c r="B32" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>15.8</v>
+      </c>
+      <c r="B33" t="n">
+        <v>15.8</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>15.6</v>
+      </c>
+      <c r="B34" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>15.8</v>
+      </c>
+      <c r="B35" t="n">
+        <v>15.8</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>15.6</v>
+      </c>
+      <c r="B36" t="n">
+        <v>16.4</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>15.8</v>
+      </c>
+      <c r="B37" t="n">
+        <v>16.2</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>16</v>
+      </c>
+      <c r="B38" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>15.8</v>
+      </c>
+      <c r="B39" t="n">
+        <v>16.6</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>16.4</v>
+      </c>
+      <c r="B40" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>16.2</v>
+      </c>
+      <c r="B41" t="n">
+        <v>16.6</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>16.4</v>
+      </c>
+      <c r="B42" t="n">
+        <v>16.8</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>16.6</v>
+      </c>
+      <c r="B43" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>16.8</v>
+      </c>
+      <c r="B44" t="n">
+        <v>17.2</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>17</v>
+      </c>
+      <c r="B45" t="n">
+        <v>17.4</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>17.2</v>
+      </c>
+      <c r="B46" t="n">
+        <v>17.2</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>17</v>
+      </c>
+      <c r="B47" t="n">
+        <v>17.4</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>17.2</v>
+      </c>
+      <c r="B48" t="n">
+        <v>17.2</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>17.4</v>
+      </c>
+      <c r="B49" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>17.2</v>
+      </c>
+      <c r="B50" t="n">
+        <v>17.2</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>17</v>
+      </c>
+      <c r="B51" t="n">
+        <v>17.4</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>16.8</v>
+      </c>
+      <c r="B52" t="n">
+        <v>17.6</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="n">
+        <v>17</v>
+      </c>
+      <c r="B53" t="n">
+        <v>17.4</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="n">
+        <v>16.8</v>
+      </c>
+      <c r="B54" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>17</v>
+      </c>
+      <c r="B55" t="n">
+        <v>17.8</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>17.2</v>
+      </c>
+      <c r="B56" t="n">
+        <v>17.6</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="n">
+        <v>17</v>
+      </c>
+      <c r="B57" t="n">
+        <v>17.4</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="n">
+        <v>17.2</v>
+      </c>
+      <c r="B58" t="n">
+        <v>17.6</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="n">
+        <v>17</v>
+      </c>
+      <c r="B59" t="n">
+        <v>17.8</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="n">
+        <v>16.8</v>
+      </c>
+      <c r="B60" t="n">
+        <v>17.6</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="n">
+        <v>17</v>
+      </c>
+      <c r="B61" t="n">
+        <v>17.4</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="n">
+        <v>17.2</v>
+      </c>
+      <c r="B62" t="n">
+        <v>17.2</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="n">
+        <v>17</v>
+      </c>
+      <c r="B63" t="n">
+        <v>17.4</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="n">
+        <v>16.8</v>
+      </c>
+      <c r="B64" t="n">
+        <v>17.6</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="n">
+        <v>17</v>
+      </c>
+      <c r="B65" t="n">
+        <v>17.4</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="n">
+        <v>16.8</v>
+      </c>
+      <c r="B66" t="n">
+        <v>17.6</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="n">
+        <v>17</v>
+      </c>
+      <c r="B67" t="n">
+        <v>17.4</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="n">
+        <v>16.4</v>
+      </c>
+      <c r="B68" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="n">
+        <v>16.6</v>
+      </c>
+      <c r="B69" t="n">
+        <v>17.8</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="n">
+        <v>16.8</v>
+      </c>
+      <c r="B70" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="n">
+        <v>17</v>
+      </c>
+      <c r="B71" t="n">
+        <v>17.8</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="n">
+        <v>17.2</v>
+      </c>
+      <c r="B72" t="n">
+        <v>17.6</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="n">
+        <v>17.4</v>
+      </c>
+      <c r="B73" t="n">
+        <v>17.8</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="n">
+        <v>16.8</v>
+      </c>
+      <c r="B74" t="n">
+        <v>18.4</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="n">
+        <v>17</v>
+      </c>
+      <c r="B75" t="n">
+        <v>18.2</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="n">
+        <v>17.2</v>
+      </c>
+      <c r="B76" t="n">
+        <v>18.4</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="n">
+        <v>17</v>
+      </c>
+      <c r="B77" t="n">
+        <v>18.6</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="n">
+        <v>17.2</v>
+      </c>
+      <c r="B78" t="n">
+        <v>18.4</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="n">
+        <v>17.4</v>
+      </c>
+      <c r="B79" t="n">
+        <v>18.6</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="n">
+        <v>17.2</v>
+      </c>
+      <c r="B80" t="n">
+        <v>18.4</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="n">
+        <v>17.4</v>
+      </c>
+      <c r="B81" t="n">
+        <v>18.2</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="n">
+        <v>17.2</v>
+      </c>
+      <c r="B82" t="n">
+        <v>18.4</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="n">
+        <v>17.4</v>
+      </c>
+      <c r="B83" t="n">
+        <v>18.2</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="n">
+        <v>17.2</v>
+      </c>
+      <c r="B84" t="n">
+        <v>18.4</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="n">
+        <v>17</v>
+      </c>
+      <c r="B85" t="n">
+        <v>18.2</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="n">
+        <v>17.2</v>
+      </c>
+      <c r="B86" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="n">
+        <v>17</v>
+      </c>
+      <c r="B87" t="n">
+        <v>18.2</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="n">
+        <v>17.2</v>
+      </c>
+      <c r="B88" t="n">
+        <v>18.4</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="n">
+        <v>17.4</v>
+      </c>
+      <c r="B89" t="n">
+        <v>18.2</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="n">
+        <v>17.2</v>
+      </c>
+      <c r="B90" t="n">
+        <v>18.4</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="n">
+        <v>17.8</v>
+      </c>
+      <c r="B91" t="n">
+        <v>17.8</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="n">
+        <v>17.6</v>
+      </c>
+      <c r="B92" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="n">
+        <v>17.4</v>
+      </c>
+      <c r="B93" t="n">
+        <v>18.2</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="n">
+        <v>18</v>
+      </c>
+      <c r="B94" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="n">
+        <v>17.8</v>
+      </c>
+      <c r="B95" t="n">
+        <v>18.2</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="n">
+        <v>17.6</v>
+      </c>
+      <c r="B96" t="n">
+        <v>18.4</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="n">
+        <v>17.8</v>
+      </c>
+      <c r="B97" t="n">
+        <v>17.8</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="n">
+        <v>17.6</v>
+      </c>
+      <c r="B98" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="n">
+        <v>17.8</v>
+      </c>
+      <c r="B99" t="n">
+        <v>17.8</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="n">
+        <v>17.6</v>
+      </c>
+      <c r="B100" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="n">
+        <v>17.4</v>
+      </c>
+      <c r="B101" t="n">
+        <v>17.8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed bug caused by having a drought or famine cause 100 percent production loss
</commit_message>
<xml_diff>
--- a/simulationdata.xlsx
+++ b/simulationdata.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B101"/>
+  <dimension ref="A1:C54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -444,21 +444,32 @@
           <t>average water price</t>
         </is>
       </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>average price</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
+        <v>5.2</v>
+      </c>
+      <c r="B2" t="n">
         <v>5.6</v>
       </c>
-      <c r="B2" t="n">
-        <v>4.8</v>
+      <c r="C2" t="n">
+        <v>5.4</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
+        <v>6.2</v>
+      </c>
+      <c r="B3" t="n">
         <v>5.4</v>
       </c>
-      <c r="B3" t="n">
-        <v>5.8</v>
+      <c r="C3" t="n">
+        <v>5.800000000000001</v>
       </c>
     </row>
     <row r="4">
@@ -468,13 +479,19 @@
       <c r="B4" t="n">
         <v>6</v>
       </c>
+      <c r="C4" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
         <v>6.6</v>
       </c>
       <c r="B5" t="n">
-        <v>6.2</v>
+        <v>5.8</v>
+      </c>
+      <c r="C5" t="n">
+        <v>6.199999999999999</v>
       </c>
     </row>
     <row r="6">
@@ -482,7 +499,10 @@
         <v>6.8</v>
       </c>
       <c r="B6" t="n">
-        <v>6.8</v>
+        <v>6.4</v>
+      </c>
+      <c r="C6" t="n">
+        <v>6.6</v>
       </c>
     </row>
     <row r="7">
@@ -490,6 +510,9 @@
         <v>7.4</v>
       </c>
       <c r="B7" t="n">
+        <v>6.6</v>
+      </c>
+      <c r="C7" t="n">
         <v>7</v>
       </c>
     </row>
@@ -498,15 +521,21 @@
         <v>7.6</v>
       </c>
       <c r="B8" t="n">
-        <v>7.6</v>
+        <v>6.8</v>
+      </c>
+      <c r="C8" t="n">
+        <v>7.199999999999999</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>8.199999999999999</v>
+        <v>7.8</v>
       </c>
       <c r="B9" t="n">
-        <v>7.8</v>
+        <v>7.4</v>
+      </c>
+      <c r="C9" t="n">
+        <v>7.6</v>
       </c>
     </row>
     <row r="10">
@@ -514,7 +543,10 @@
         <v>8.4</v>
       </c>
       <c r="B10" t="n">
-        <v>8.4</v>
+        <v>7.6</v>
+      </c>
+      <c r="C10" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="11">
@@ -522,38 +554,53 @@
         <v>8.6</v>
       </c>
       <c r="B11" t="n">
-        <v>9</v>
+        <v>8.199999999999999</v>
+      </c>
+      <c r="C11" t="n">
+        <v>8.399999999999999</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>9.199999999999999</v>
+        <v>8.800000000000001</v>
       </c>
       <c r="B12" t="n">
         <v>8.800000000000001</v>
       </c>
+      <c r="C12" t="n">
+        <v>8.800000000000001</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
+        <v>9</v>
+      </c>
+      <c r="B13" t="n">
         <v>9.4</v>
       </c>
-      <c r="B13" t="n">
-        <v>9</v>
+      <c r="C13" t="n">
+        <v>9.199999999999999</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>10</v>
+        <v>9.6</v>
       </c>
       <c r="B14" t="n">
         <v>9.199999999999999</v>
       </c>
+      <c r="C14" t="n">
+        <v>9.4</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>10.2</v>
+        <v>9.800000000000001</v>
       </c>
       <c r="B15" t="n">
+        <v>9.800000000000001</v>
+      </c>
+      <c r="C15" t="n">
         <v>9.800000000000001</v>
       </c>
     </row>
@@ -562,15 +609,21 @@
         <v>10.4</v>
       </c>
       <c r="B16" t="n">
-        <v>10.4</v>
+        <v>10</v>
+      </c>
+      <c r="C16" t="n">
+        <v>10.2</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>11</v>
+        <v>10.6</v>
       </c>
       <c r="B17" t="n">
-        <v>10.6</v>
+        <v>10.2</v>
+      </c>
+      <c r="C17" t="n">
+        <v>10.4</v>
       </c>
     </row>
     <row r="18">
@@ -578,23 +631,32 @@
         <v>11.2</v>
       </c>
       <c r="B18" t="n">
-        <v>11.2</v>
+        <v>10.4</v>
+      </c>
+      <c r="C18" t="n">
+        <v>10.8</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>11.8</v>
+        <v>11.4</v>
       </c>
       <c r="B19" t="n">
-        <v>11.4</v>
+        <v>11</v>
+      </c>
+      <c r="C19" t="n">
+        <v>11.2</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>12</v>
+        <v>11.6</v>
       </c>
       <c r="B20" t="n">
-        <v>12</v>
+        <v>11.6</v>
+      </c>
+      <c r="C20" t="n">
+        <v>11.6</v>
       </c>
     </row>
     <row r="21">
@@ -602,15 +664,21 @@
         <v>12.2</v>
       </c>
       <c r="B21" t="n">
-        <v>12.6</v>
+        <v>11.8</v>
+      </c>
+      <c r="C21" t="n">
+        <v>12</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
+        <v>12</v>
+      </c>
+      <c r="B22" t="n">
         <v>12.4</v>
       </c>
-      <c r="B22" t="n">
-        <v>12.8</v>
+      <c r="C22" t="n">
+        <v>12.2</v>
       </c>
     </row>
     <row r="23">
@@ -618,7 +686,10 @@
         <v>12.6</v>
       </c>
       <c r="B23" t="n">
-        <v>13</v>
+        <v>12.6</v>
+      </c>
+      <c r="C23" t="n">
+        <v>12.6</v>
       </c>
     </row>
     <row r="24">
@@ -626,7 +697,10 @@
         <v>12.8</v>
       </c>
       <c r="B24" t="n">
-        <v>13.6</v>
+        <v>13.2</v>
+      </c>
+      <c r="C24" t="n">
+        <v>13</v>
       </c>
     </row>
     <row r="25">
@@ -634,7 +708,10 @@
         <v>13.4</v>
       </c>
       <c r="B25" t="n">
-        <v>13.8</v>
+        <v>13</v>
+      </c>
+      <c r="C25" t="n">
+        <v>13.2</v>
       </c>
     </row>
     <row r="26">
@@ -642,63 +719,87 @@
         <v>13.6</v>
       </c>
       <c r="B26" t="n">
-        <v>14.4</v>
+        <v>13.2</v>
+      </c>
+      <c r="C26" t="n">
+        <v>13.4</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>14.2</v>
+        <v>13.8</v>
       </c>
       <c r="B27" t="n">
-        <v>14.6</v>
+        <v>13.4</v>
+      </c>
+      <c r="C27" t="n">
+        <v>13.6</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>14.4</v>
+        <v>14</v>
       </c>
       <c r="B28" t="n">
-        <v>14.8</v>
+        <v>13.6</v>
+      </c>
+      <c r="C28" t="n">
+        <v>13.8</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>14.6</v>
+        <v>14.2</v>
       </c>
       <c r="B29" t="n">
-        <v>15</v>
+        <v>13.8</v>
+      </c>
+      <c r="C29" t="n">
+        <v>14</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>14.8</v>
+        <v>14.4</v>
       </c>
       <c r="B30" t="n">
-        <v>15.2</v>
+        <v>14.4</v>
+      </c>
+      <c r="C30" t="n">
+        <v>14.4</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
+        <v>14.6</v>
+      </c>
+      <c r="B31" t="n">
         <v>15</v>
       </c>
-      <c r="B31" t="n">
-        <v>15.8</v>
+      <c r="C31" t="n">
+        <v>14.8</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
+        <v>14.8</v>
+      </c>
+      <c r="B32" t="n">
         <v>15.2</v>
       </c>
-      <c r="B32" t="n">
-        <v>16</v>
+      <c r="C32" t="n">
+        <v>15</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>15.8</v>
+        <v>15.4</v>
       </c>
       <c r="B33" t="n">
-        <v>15.8</v>
+        <v>15</v>
+      </c>
+      <c r="C33" t="n">
+        <v>15.2</v>
       </c>
     </row>
     <row r="34">
@@ -706,7 +807,10 @@
         <v>15.6</v>
       </c>
       <c r="B34" t="n">
-        <v>16</v>
+        <v>15.2</v>
+      </c>
+      <c r="C34" t="n">
+        <v>15.4</v>
       </c>
     </row>
     <row r="35">
@@ -714,55 +818,76 @@
         <v>15.8</v>
       </c>
       <c r="B35" t="n">
-        <v>15.8</v>
+        <v>15.4</v>
+      </c>
+      <c r="C35" t="n">
+        <v>15.6</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
+        <v>16</v>
+      </c>
+      <c r="B36" t="n">
         <v>15.6</v>
       </c>
-      <c r="B36" t="n">
-        <v>16.4</v>
+      <c r="C36" t="n">
+        <v>15.8</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
+        <v>16.2</v>
+      </c>
+      <c r="B37" t="n">
+        <v>15.4</v>
+      </c>
+      <c r="C37" t="n">
         <v>15.8</v>
-      </c>
-      <c r="B37" t="n">
-        <v>16.2</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>16</v>
+        <v>16.4</v>
       </c>
       <c r="B38" t="n">
-        <v>16</v>
+        <v>15.2</v>
+      </c>
+      <c r="C38" t="n">
+        <v>15.8</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
+        <v>16.2</v>
+      </c>
+      <c r="B39" t="n">
         <v>15.8</v>
       </c>
-      <c r="B39" t="n">
-        <v>16.6</v>
+      <c r="C39" t="n">
+        <v>16</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>16.4</v>
+        <v>16.8</v>
       </c>
       <c r="B40" t="n">
-        <v>16</v>
+        <v>15.6</v>
+      </c>
+      <c r="C40" t="n">
+        <v>16.2</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
+        <v>16.6</v>
+      </c>
+      <c r="B41" t="n">
+        <v>15.8</v>
+      </c>
+      <c r="C41" t="n">
         <v>16.2</v>
-      </c>
-      <c r="B41" t="n">
-        <v>16.6</v>
       </c>
     </row>
     <row r="42">
@@ -770,15 +895,21 @@
         <v>16.4</v>
       </c>
       <c r="B42" t="n">
-        <v>16.8</v>
+        <v>16</v>
+      </c>
+      <c r="C42" t="n">
+        <v>16.2</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>16.6</v>
+        <v>17</v>
       </c>
       <c r="B43" t="n">
-        <v>17</v>
+        <v>15.8</v>
+      </c>
+      <c r="C43" t="n">
+        <v>16.4</v>
       </c>
     </row>
     <row r="44">
@@ -786,7 +917,10 @@
         <v>16.8</v>
       </c>
       <c r="B44" t="n">
-        <v>17.2</v>
+        <v>16.4</v>
+      </c>
+      <c r="C44" t="n">
+        <v>16.6</v>
       </c>
     </row>
     <row r="45">
@@ -794,15 +928,21 @@
         <v>17</v>
       </c>
       <c r="B45" t="n">
-        <v>17.4</v>
+        <v>16.2</v>
+      </c>
+      <c r="C45" t="n">
+        <v>16.6</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>17.2</v>
+        <v>16.8</v>
       </c>
       <c r="B46" t="n">
-        <v>17.2</v>
+        <v>16.4</v>
+      </c>
+      <c r="C46" t="n">
+        <v>16.6</v>
       </c>
     </row>
     <row r="47">
@@ -810,23 +950,32 @@
         <v>17</v>
       </c>
       <c r="B47" t="n">
-        <v>17.4</v>
+        <v>16.2</v>
+      </c>
+      <c r="C47" t="n">
+        <v>16.6</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>17.2</v>
+        <v>16.8</v>
       </c>
       <c r="B48" t="n">
-        <v>17.2</v>
+        <v>16.4</v>
+      </c>
+      <c r="C48" t="n">
+        <v>16.6</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>17.4</v>
+        <v>17</v>
       </c>
       <c r="B49" t="n">
-        <v>17</v>
+        <v>16.6</v>
+      </c>
+      <c r="C49" t="n">
+        <v>16.8</v>
       </c>
     </row>
     <row r="50">
@@ -834,415 +983,54 @@
         <v>17.2</v>
       </c>
       <c r="B50" t="n">
-        <v>17.2</v>
+        <v>16.4</v>
+      </c>
+      <c r="C50" t="n">
+        <v>16.8</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
+        <v>17.8</v>
+      </c>
+      <c r="B51" t="n">
+        <v>16.2</v>
+      </c>
+      <c r="C51" t="n">
         <v>17</v>
-      </c>
-      <c r="B51" t="n">
-        <v>17.4</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
+        <v>17.6</v>
+      </c>
+      <c r="B52" t="n">
         <v>16.8</v>
       </c>
-      <c r="B52" t="n">
-        <v>17.6</v>
+      <c r="C52" t="n">
+        <v>17.2</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>17</v>
+        <v>17.8</v>
       </c>
       <c r="B53" t="n">
-        <v>17.4</v>
+        <v>16.6</v>
+      </c>
+      <c r="C53" t="n">
+        <v>17.2</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
+        <v>17.6</v>
+      </c>
+      <c r="B54" t="n">
         <v>16.8</v>
       </c>
-      <c r="B54" t="n">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" t="n">
-        <v>17</v>
-      </c>
-      <c r="B55" t="n">
-        <v>17.8</v>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" t="n">
+      <c r="C54" t="n">
         <v>17.2</v>
-      </c>
-      <c r="B56" t="n">
-        <v>17.6</v>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" t="n">
-        <v>17</v>
-      </c>
-      <c r="B57" t="n">
-        <v>17.4</v>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58" t="n">
-        <v>17.2</v>
-      </c>
-      <c r="B58" t="n">
-        <v>17.6</v>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59" t="n">
-        <v>17</v>
-      </c>
-      <c r="B59" t="n">
-        <v>17.8</v>
-      </c>
-    </row>
-    <row r="60">
-      <c r="A60" t="n">
-        <v>16.8</v>
-      </c>
-      <c r="B60" t="n">
-        <v>17.6</v>
-      </c>
-    </row>
-    <row r="61">
-      <c r="A61" t="n">
-        <v>17</v>
-      </c>
-      <c r="B61" t="n">
-        <v>17.4</v>
-      </c>
-    </row>
-    <row r="62">
-      <c r="A62" t="n">
-        <v>17.2</v>
-      </c>
-      <c r="B62" t="n">
-        <v>17.2</v>
-      </c>
-    </row>
-    <row r="63">
-      <c r="A63" t="n">
-        <v>17</v>
-      </c>
-      <c r="B63" t="n">
-        <v>17.4</v>
-      </c>
-    </row>
-    <row r="64">
-      <c r="A64" t="n">
-        <v>16.8</v>
-      </c>
-      <c r="B64" t="n">
-        <v>17.6</v>
-      </c>
-    </row>
-    <row r="65">
-      <c r="A65" t="n">
-        <v>17</v>
-      </c>
-      <c r="B65" t="n">
-        <v>17.4</v>
-      </c>
-    </row>
-    <row r="66">
-      <c r="A66" t="n">
-        <v>16.8</v>
-      </c>
-      <c r="B66" t="n">
-        <v>17.6</v>
-      </c>
-    </row>
-    <row r="67">
-      <c r="A67" t="n">
-        <v>17</v>
-      </c>
-      <c r="B67" t="n">
-        <v>17.4</v>
-      </c>
-    </row>
-    <row r="68">
-      <c r="A68" t="n">
-        <v>16.4</v>
-      </c>
-      <c r="B68" t="n">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="69">
-      <c r="A69" t="n">
-        <v>16.6</v>
-      </c>
-      <c r="B69" t="n">
-        <v>17.8</v>
-      </c>
-    </row>
-    <row r="70">
-      <c r="A70" t="n">
-        <v>16.8</v>
-      </c>
-      <c r="B70" t="n">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="71">
-      <c r="A71" t="n">
-        <v>17</v>
-      </c>
-      <c r="B71" t="n">
-        <v>17.8</v>
-      </c>
-    </row>
-    <row r="72">
-      <c r="A72" t="n">
-        <v>17.2</v>
-      </c>
-      <c r="B72" t="n">
-        <v>17.6</v>
-      </c>
-    </row>
-    <row r="73">
-      <c r="A73" t="n">
-        <v>17.4</v>
-      </c>
-      <c r="B73" t="n">
-        <v>17.8</v>
-      </c>
-    </row>
-    <row r="74">
-      <c r="A74" t="n">
-        <v>16.8</v>
-      </c>
-      <c r="B74" t="n">
-        <v>18.4</v>
-      </c>
-    </row>
-    <row r="75">
-      <c r="A75" t="n">
-        <v>17</v>
-      </c>
-      <c r="B75" t="n">
-        <v>18.2</v>
-      </c>
-    </row>
-    <row r="76">
-      <c r="A76" t="n">
-        <v>17.2</v>
-      </c>
-      <c r="B76" t="n">
-        <v>18.4</v>
-      </c>
-    </row>
-    <row r="77">
-      <c r="A77" t="n">
-        <v>17</v>
-      </c>
-      <c r="B77" t="n">
-        <v>18.6</v>
-      </c>
-    </row>
-    <row r="78">
-      <c r="A78" t="n">
-        <v>17.2</v>
-      </c>
-      <c r="B78" t="n">
-        <v>18.4</v>
-      </c>
-    </row>
-    <row r="79">
-      <c r="A79" t="n">
-        <v>17.4</v>
-      </c>
-      <c r="B79" t="n">
-        <v>18.6</v>
-      </c>
-    </row>
-    <row r="80">
-      <c r="A80" t="n">
-        <v>17.2</v>
-      </c>
-      <c r="B80" t="n">
-        <v>18.4</v>
-      </c>
-    </row>
-    <row r="81">
-      <c r="A81" t="n">
-        <v>17.4</v>
-      </c>
-      <c r="B81" t="n">
-        <v>18.2</v>
-      </c>
-    </row>
-    <row r="82">
-      <c r="A82" t="n">
-        <v>17.2</v>
-      </c>
-      <c r="B82" t="n">
-        <v>18.4</v>
-      </c>
-    </row>
-    <row r="83">
-      <c r="A83" t="n">
-        <v>17.4</v>
-      </c>
-      <c r="B83" t="n">
-        <v>18.2</v>
-      </c>
-    </row>
-    <row r="84">
-      <c r="A84" t="n">
-        <v>17.2</v>
-      </c>
-      <c r="B84" t="n">
-        <v>18.4</v>
-      </c>
-    </row>
-    <row r="85">
-      <c r="A85" t="n">
-        <v>17</v>
-      </c>
-      <c r="B85" t="n">
-        <v>18.2</v>
-      </c>
-    </row>
-    <row r="86">
-      <c r="A86" t="n">
-        <v>17.2</v>
-      </c>
-      <c r="B86" t="n">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="87">
-      <c r="A87" t="n">
-        <v>17</v>
-      </c>
-      <c r="B87" t="n">
-        <v>18.2</v>
-      </c>
-    </row>
-    <row r="88">
-      <c r="A88" t="n">
-        <v>17.2</v>
-      </c>
-      <c r="B88" t="n">
-        <v>18.4</v>
-      </c>
-    </row>
-    <row r="89">
-      <c r="A89" t="n">
-        <v>17.4</v>
-      </c>
-      <c r="B89" t="n">
-        <v>18.2</v>
-      </c>
-    </row>
-    <row r="90">
-      <c r="A90" t="n">
-        <v>17.2</v>
-      </c>
-      <c r="B90" t="n">
-        <v>18.4</v>
-      </c>
-    </row>
-    <row r="91">
-      <c r="A91" t="n">
-        <v>17.8</v>
-      </c>
-      <c r="B91" t="n">
-        <v>17.8</v>
-      </c>
-    </row>
-    <row r="92">
-      <c r="A92" t="n">
-        <v>17.6</v>
-      </c>
-      <c r="B92" t="n">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="93">
-      <c r="A93" t="n">
-        <v>17.4</v>
-      </c>
-      <c r="B93" t="n">
-        <v>18.2</v>
-      </c>
-    </row>
-    <row r="94">
-      <c r="A94" t="n">
-        <v>18</v>
-      </c>
-      <c r="B94" t="n">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="95">
-      <c r="A95" t="n">
-        <v>17.8</v>
-      </c>
-      <c r="B95" t="n">
-        <v>18.2</v>
-      </c>
-    </row>
-    <row r="96">
-      <c r="A96" t="n">
-        <v>17.6</v>
-      </c>
-      <c r="B96" t="n">
-        <v>18.4</v>
-      </c>
-    </row>
-    <row r="97">
-      <c r="A97" t="n">
-        <v>17.8</v>
-      </c>
-      <c r="B97" t="n">
-        <v>17.8</v>
-      </c>
-    </row>
-    <row r="98">
-      <c r="A98" t="n">
-        <v>17.6</v>
-      </c>
-      <c r="B98" t="n">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="99">
-      <c r="A99" t="n">
-        <v>17.8</v>
-      </c>
-      <c r="B99" t="n">
-        <v>17.8</v>
-      </c>
-    </row>
-    <row r="100">
-      <c r="A100" t="n">
-        <v>17.6</v>
-      </c>
-      <c r="B100" t="n">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="101">
-      <c r="A101" t="n">
-        <v>17.4</v>
-      </c>
-      <c r="B101" t="n">
-        <v>17.8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>